<commit_message>
updated diary entries 1/19/20
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/Diaries/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/SWE265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306D568C-1AE1-4E42-8C06-A06E05C911B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ED9E86-9604-BE4F-8DD2-46703F87A891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="3380" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -78,16 +78,82 @@
     <t>Learning to read code is much more valuable than I thought.</t>
   </si>
   <si>
-    <t>5:00 -7:50</t>
-  </si>
-  <si>
     <t>I was able to set up the environments and get two of the three open source applications to run</t>
   </si>
   <si>
     <t>Slightly overwhelmed when Jedit wasn't working but also excited to learn how to navigate open source applications.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>3:00 - 5:00 pm</t>
+  </si>
+  <si>
+    <t>Rafael, Jay, Chris</t>
+  </si>
+  <si>
+    <t>We compiled a list of 10 projects that looed intersing. We were ablt to decide on one after class ended</t>
+  </si>
+  <si>
+    <t>Finding an open source project that is not a library or a framework and in Java was more challenging than I thought it would be.</t>
+  </si>
+  <si>
+    <t>We were able to fnd bugs and fix pacman 1-2</t>
+  </si>
+  <si>
+    <t>Pacman 1-3, learn reverse engineering and design methods</t>
+  </si>
+  <si>
+    <t>Going through the source code with class made the process of searrching/reading through source code a lot more fun than if I were to do it alone. I think if I had done it alone it would have taken much longer</t>
+  </si>
+  <si>
+    <t>I found an open source project but ran into several issues trying to get it to run on my computer</t>
+  </si>
+  <si>
+    <t>I assumed I could just open a project from github through IntelliJ without reading instructions in the ReadMe. I learned that I should definitely read through before downloading.</t>
+  </si>
+  <si>
+    <t>2:00 - 3:00 pm</t>
+  </si>
+  <si>
+    <t>5:00 -7:50 pm</t>
+  </si>
+  <si>
+    <t>12:00 - 2:00 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacman 3: find rule for how cyan ghost moves and make pacman move by 2 </t>
+  </si>
+  <si>
+    <t>I was able to find the rues for how the cyan ghost moves</t>
+  </si>
+  <si>
+    <t>Finding the rules for the ghost was fairly straightforward. Trying to make pacman move by 2 steps at a time proved to be more challening for me. I felt like it was a very circuious process of going through one folder then another. Not sure if it was more challenging because I was doing it by myself or if finding the rule for pacman was harder than the other problems</t>
+  </si>
+  <si>
+    <t>Frustrated</t>
+  </si>
+  <si>
+    <t>Find a third open source project for hw</t>
+  </si>
+  <si>
+    <t>Find an opensource project for group project</t>
+  </si>
+  <si>
+    <t>Fun/good</t>
+  </si>
+  <si>
+    <t>Fun &amp; challeneged</t>
+  </si>
+  <si>
+    <t>2:00 - 4:00 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacman3 HW </t>
+  </si>
+  <si>
+    <t>Was able to complete homework</t>
+  </si>
+  <si>
+    <t>Learning how to integrate fruit into pacman was fun. I felt like I really had to dive into the code and get a good undertanding for how all pieces in the game should interact</t>
   </si>
 </sst>
 </file>
@@ -232,7 +298,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -258,9 +324,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -272,6 +335,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -591,39 +666,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" style="16" customWidth="1"/>
+    <col min="2" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -632,7 +708,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -645,10 +721,10 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
@@ -658,7 +734,7 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -671,7 +747,7 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -680,7 +756,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -712,11 +788,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>43839</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>17</v>
+      <c r="B10" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>14</v>
@@ -725,131 +801,159 @@
         <v>15</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>43842</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>43846</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
+      <c r="D12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>43846</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>43848</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>43849</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -858,7 +962,7 @@
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
@@ -867,16 +971,16 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -885,7 +989,7 @@
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -894,7 +998,7 @@
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -903,7 +1007,7 @@
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -912,7 +1016,7 @@
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -921,7 +1025,7 @@
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -930,7 +1034,7 @@
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -939,7 +1043,7 @@
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -948,7 +1052,7 @@
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -957,7 +1061,7 @@
       <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -966,7 +1070,7 @@
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -975,7 +1079,7 @@
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -984,7 +1088,7 @@
       <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -993,7 +1097,7 @@
       <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1002,7 +1106,7 @@
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1011,7 +1115,7 @@
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1020,7 +1124,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1029,7 +1133,7 @@
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1038,7 +1142,7 @@
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
+      <c r="A40" s="11"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -1047,7 +1151,7 @@
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -1056,7 +1160,7 @@
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -1065,7 +1169,7 @@
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -1074,7 +1178,7 @@
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -1083,7 +1187,7 @@
       <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -1092,7 +1196,7 @@
       <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
+      <c r="A46" s="11"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -1101,7 +1205,7 @@
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -1110,7 +1214,7 @@
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
+      <c r="A48" s="11"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -1119,7 +1223,7 @@
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -1128,7 +1232,7 @@
       <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -1137,7 +1241,7 @@
       <c r="G50" s="8"/>
     </row>
     <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="7"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -1146,7 +1250,7 @@
       <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -1155,7 +1259,7 @@
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="7"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -1164,7 +1268,7 @@
       <c r="G53" s="8"/>
     </row>
     <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -1173,7 +1277,7 @@
       <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="7"/>
+      <c r="A55" s="11"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -1182,7 +1286,7 @@
       <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
+      <c r="A56" s="11"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -1191,7 +1295,7 @@
       <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="7"/>
+      <c r="A57" s="11"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -1200,7 +1304,7 @@
       <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="7"/>
+      <c r="A58" s="11"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -1209,7 +1313,7 @@
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="7"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -1218,7 +1322,7 @@
       <c r="G59" s="8"/>
     </row>
     <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="7"/>
+      <c r="A60" s="11"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -1227,7 +1331,7 @@
       <c r="G60" s="8"/>
     </row>
     <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="7"/>
+      <c r="A61" s="11"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -1236,7 +1340,7 @@
       <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="7"/>
+      <c r="A62" s="11"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -1245,7 +1349,7 @@
       <c r="G62" s="8"/>
     </row>
     <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="7"/>
+      <c r="A63" s="11"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -1254,7 +1358,7 @@
       <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="7"/>
+      <c r="A64" s="11"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -1263,7 +1367,7 @@
       <c r="G64" s="8"/>
     </row>
     <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="7"/>
+      <c r="A65" s="11"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -1272,7 +1376,7 @@
       <c r="G65" s="8"/>
     </row>
     <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="7"/>
+      <c r="A66" s="11"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -1281,7 +1385,7 @@
       <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="7"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -1290,7 +1394,7 @@
       <c r="G67" s="8"/>
     </row>
     <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="7"/>
+      <c r="A68" s="11"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -1299,7 +1403,7 @@
       <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="7"/>
+      <c r="A69" s="11"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -1308,7 +1412,7 @@
       <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="7"/>
+      <c r="A70" s="11"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -1317,7 +1421,7 @@
       <c r="G70" s="8"/>
     </row>
     <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="7"/>
+      <c r="A71" s="11"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -1326,7 +1430,7 @@
       <c r="G71" s="8"/>
     </row>
     <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="7"/>
+      <c r="A72" s="11"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -1335,7 +1439,7 @@
       <c r="G72" s="8"/>
     </row>
     <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="7"/>
+      <c r="A73" s="11"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -1344,7 +1448,7 @@
       <c r="G73" s="8"/>
     </row>
     <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="7"/>
+      <c r="A74" s="11"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -1353,7 +1457,7 @@
       <c r="G74" s="8"/>
     </row>
     <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="7"/>
+      <c r="A75" s="11"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -1362,7 +1466,7 @@
       <c r="G75" s="8"/>
     </row>
     <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="7"/>
+      <c r="A76" s="11"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -1371,7 +1475,7 @@
       <c r="G76" s="8"/>
     </row>
     <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="7"/>
+      <c r="A77" s="11"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -1380,7 +1484,7 @@
       <c r="G77" s="8"/>
     </row>
     <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="7"/>
+      <c r="A78" s="11"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -1389,7 +1493,7 @@
       <c r="G78" s="8"/>
     </row>
     <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="7"/>
+      <c r="A79" s="11"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -1398,7 +1502,7 @@
       <c r="G79" s="8"/>
     </row>
     <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="7"/>
+      <c r="A80" s="11"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -1407,7 +1511,7 @@
       <c r="G80" s="8"/>
     </row>
     <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="7"/>
+      <c r="A81" s="11"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -1416,7 +1520,7 @@
       <c r="G81" s="8"/>
     </row>
     <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="7"/>
+      <c r="A82" s="11"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -1425,7 +1529,7 @@
       <c r="G82" s="8"/>
     </row>
     <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="7"/>
+      <c r="A83" s="11"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -1434,7 +1538,7 @@
       <c r="G83" s="8"/>
     </row>
     <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="7"/>
+      <c r="A84" s="11"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -1443,7 +1547,7 @@
       <c r="G84" s="8"/>
     </row>
     <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="7"/>
+      <c r="A85" s="11"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -1452,7 +1556,7 @@
       <c r="G85" s="8"/>
     </row>
     <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="7"/>
+      <c r="A86" s="11"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
@@ -1461,7 +1565,7 @@
       <c r="G86" s="8"/>
     </row>
     <row r="87" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="7"/>
+      <c r="A87" s="11"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
@@ -1470,7 +1574,7 @@
       <c r="G87" s="8"/>
     </row>
     <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="7"/>
+      <c r="A88" s="11"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -1479,7 +1583,7 @@
       <c r="G88" s="8"/>
     </row>
     <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="7"/>
+      <c r="A89" s="11"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -1488,7 +1592,7 @@
       <c r="G89" s="8"/>
     </row>
     <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="7"/>
+      <c r="A90" s="11"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -1497,7 +1601,7 @@
       <c r="G90" s="8"/>
     </row>
     <row r="91" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="7"/>
+      <c r="A91" s="11"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -1506,7 +1610,7 @@
       <c r="G91" s="8"/>
     </row>
     <row r="92" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="7"/>
+      <c r="A92" s="11"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -1515,7 +1619,7 @@
       <c r="G92" s="8"/>
     </row>
     <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="7"/>
+      <c r="A93" s="11"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -1524,7 +1628,7 @@
       <c r="G93" s="8"/>
     </row>
     <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="7"/>
+      <c r="A94" s="11"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -1533,7 +1637,7 @@
       <c r="G94" s="8"/>
     </row>
     <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="7"/>
+      <c r="A95" s="11"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
@@ -1542,7 +1646,7 @@
       <c r="G95" s="8"/>
     </row>
     <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="7"/>
+      <c r="A96" s="11"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
@@ -1551,7 +1655,7 @@
       <c r="G96" s="8"/>
     </row>
     <row r="97" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A97" s="7"/>
+      <c r="A97" s="11"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
@@ -1560,7 +1664,7 @@
       <c r="G97" s="8"/>
     </row>
     <row r="98" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="7"/>
+      <c r="A98" s="11"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
@@ -1569,7 +1673,7 @@
       <c r="G98" s="8"/>
     </row>
     <row r="99" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" s="7"/>
+      <c r="A99" s="11"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
@@ -1578,7 +1682,7 @@
       <c r="G99" s="8"/>
     </row>
     <row r="100" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="7"/>
+      <c r="A100" s="11"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
@@ -1587,7 +1691,7 @@
       <c r="G100" s="8"/>
     </row>
     <row r="101" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="7"/>
+      <c r="A101" s="11"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
@@ -1596,7 +1700,7 @@
       <c r="G101" s="8"/>
     </row>
     <row r="102" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" s="7"/>
+      <c r="A102" s="11"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -1605,7 +1709,7 @@
       <c r="G102" s="8"/>
     </row>
     <row r="103" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" s="7"/>
+      <c r="A103" s="11"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
@@ -1614,7 +1718,7 @@
       <c r="G103" s="8"/>
     </row>
     <row r="104" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="7"/>
+      <c r="A104" s="11"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -1623,7 +1727,7 @@
       <c r="G104" s="8"/>
     </row>
     <row r="105" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="7"/>
+      <c r="A105" s="11"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
@@ -1632,7 +1736,7 @@
       <c r="G105" s="8"/>
     </row>
     <row r="106" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="7"/>
+      <c r="A106" s="11"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -1641,7 +1745,7 @@
       <c r="G106" s="8"/>
     </row>
     <row r="107" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" s="7"/>
+      <c r="A107" s="11"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -1650,7 +1754,7 @@
       <c r="G107" s="8"/>
     </row>
     <row r="108" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A108" s="7"/>
+      <c r="A108" s="11"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
@@ -1659,7 +1763,7 @@
       <c r="G108" s="8"/>
     </row>
     <row r="109" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="7"/>
+      <c r="A109" s="11"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
@@ -1668,7 +1772,7 @@
       <c r="G109" s="8"/>
     </row>
     <row r="110" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="7"/>
+      <c r="A110" s="11"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
@@ -1677,7 +1781,7 @@
       <c r="G110" s="8"/>
     </row>
     <row r="111" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="7"/>
+      <c r="A111" s="11"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
@@ -1686,7 +1790,7 @@
       <c r="G111" s="8"/>
     </row>
     <row r="112" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="7"/>
+      <c r="A112" s="11"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
@@ -1695,7 +1799,7 @@
       <c r="G112" s="8"/>
     </row>
     <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113" s="7"/>
+      <c r="A113" s="11"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
@@ -1704,7 +1808,7 @@
       <c r="G113" s="8"/>
     </row>
     <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="7"/>
+      <c r="A114" s="11"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
@@ -1713,7 +1817,7 @@
       <c r="G114" s="8"/>
     </row>
     <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="7"/>
+      <c r="A115" s="11"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -1722,7 +1826,7 @@
       <c r="G115" s="8"/>
     </row>
     <row r="116" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="7"/>
+      <c r="A116" s="11"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
@@ -1731,7 +1835,7 @@
       <c r="G116" s="8"/>
     </row>
     <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="7"/>
+      <c r="A117" s="11"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
@@ -1740,7 +1844,7 @@
       <c r="G117" s="8"/>
     </row>
     <row r="118" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="7"/>
+      <c r="A118" s="11"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
@@ -1749,7 +1853,7 @@
       <c r="G118" s="8"/>
     </row>
     <row r="119" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="7"/>
+      <c r="A119" s="11"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
@@ -1758,7 +1862,7 @@
       <c r="G119" s="8"/>
     </row>
     <row r="120" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="7"/>
+      <c r="A120" s="11"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
@@ -1767,7 +1871,7 @@
       <c r="G120" s="8"/>
     </row>
     <row r="121" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="7"/>
+      <c r="A121" s="11"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
@@ -1776,7 +1880,7 @@
       <c r="G121" s="8"/>
     </row>
     <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="7"/>
+      <c r="A122" s="11"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
@@ -1785,7 +1889,7 @@
       <c r="G122" s="8"/>
     </row>
     <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="7"/>
+      <c r="A123" s="11"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
@@ -1794,22 +1898,13 @@
       <c r="G123" s="8"/>
     </row>
     <row r="124" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="7"/>
+      <c r="A124" s="11"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
-    </row>
-    <row r="125" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="7"/>
-      <c r="B125" s="7"/>
-      <c r="C125" s="7"/>
-      <c r="D125" s="7"/>
-      <c r="E125" s="7"/>
-      <c r="F125" s="7"/>
-      <c r="G125" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
update diary for class and project
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/SWE265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ED9E86-9604-BE4F-8DD2-46703F87A891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EBF387-3F96-8F42-AAEC-F8FBDE48C816}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -154,6 +154,33 @@
   </si>
   <si>
     <t>Learning how to integrate fruit into pacman was fun. I felt like I really had to dive into the code and get a good undertanding for how all pieces in the game should interact</t>
+  </si>
+  <si>
+    <t>Mental Models</t>
+  </si>
+  <si>
+    <t>learn the importance of mental models and why you should externalize your thought process/diagrams of programs</t>
+  </si>
+  <si>
+    <t>I found the idea of extranlizing your mental process to be much more valuable than I had anticipated. That's defintely something I need to work on when tackling problems</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>3:00 - 7:45pm</t>
+  </si>
+  <si>
+    <t>Chris, Jay, Rafael</t>
+  </si>
+  <si>
+    <t>Work on open source project: find 2 features, print UML diagram, and writeup</t>
+  </si>
+  <si>
+    <t>We were able to accomplish our three goals tonight</t>
+  </si>
+  <si>
+    <t>Going through the source code with everyone was a pretty fun process. Filling out the template was annoying although I understand the importance of putting your thoughts on paper and backing up the decisions you make. I also realized how important it was to document your process because we relied on the template to follow back our bread crumbs. Would have been lost otherwise</t>
   </si>
 </sst>
 </file>
@@ -336,9 +363,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -347,6 +371,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -668,38 +695,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" style="15" customWidth="1"/>
     <col min="2" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -708,7 +735,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -721,7 +748,7 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -734,7 +761,7 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -747,7 +774,7 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -756,7 +783,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -925,23 +952,51 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
+    <row r="16" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>43853</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>43855</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>

</xml_diff>

<commit_message>
updated diary entries 2/1
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/SWE265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EBF387-3F96-8F42-AAEC-F8FBDE48C816}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15993992-5B2E-8945-ABA3-157011BAF1CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -181,6 +181,27 @@
   </si>
   <si>
     <t>Going through the source code with everyone was a pretty fun process. Filling out the template was annoying although I understand the importance of putting your thoughts on paper and backing up the decisions you make. I also realized how important it was to document your process because we relied on the template to follow back our bread crumbs. Would have been lost otherwise</t>
+  </si>
+  <si>
+    <t>UML relationships, overview of visual tools and diagrams.</t>
+  </si>
+  <si>
+    <t>we learned new models to read and understand code</t>
+  </si>
+  <si>
+    <t>I felt that we went over the UML diagram for a little too long and skipped over sequence graphs and call graphs too quickly. I would have liked to had more time spent on the visual tools because they seemed helpful for reading and understanding larger codebases</t>
+  </si>
+  <si>
+    <t>1:00 - 5:00pm</t>
+  </si>
+  <si>
+    <t>Work on open source project: find 2 essential features and create a packet containing everything relevant to those features</t>
+  </si>
+  <si>
+    <t>We were able to find 2 features and write a packet</t>
+  </si>
+  <si>
+    <t>I found that going thorugh the codebase to find essential features was much easier now that I was familiar with the program. It was nice knowing where to search and using call graphs to sift through relveant methods and classes</t>
   </si>
 </sst>
 </file>
@@ -325,7 +346,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -374,6 +395,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -695,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -998,23 +1022,51 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
+    <row r="18" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>43860</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A19" s="17">
+        <v>43862</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>

</xml_diff>

<commit_message>
updated diary entry 2/10
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/SWE265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15993992-5B2E-8945-ABA3-157011BAF1CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C77C84-4974-8545-9C37-B428A5A3FA88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>I found that going thorugh the codebase to find essential features was much easier now that I was familiar with the program. It was nice knowing where to search and using call graphs to sift through relveant methods and classes</t>
+  </si>
+  <si>
+    <t>Mental Simulations, walking through code</t>
+  </si>
+  <si>
+    <t>We learned new methods for thining in different mental models and walking through code in an efficient manner</t>
+  </si>
+  <si>
+    <t>I really liked the guest speaker - he opened me up on how you can really reuse your own software to sell to new clients. I also enjoyed walking through code and exteranlizing my thoughts to my partner during the code exercises. Shows that you can have an idea about how something works but communicating it is a whole different matter</t>
   </si>
 </sst>
 </file>
@@ -393,11 +402,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -719,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -730,24 +739,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
@@ -1046,7 +1055,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A19" s="17">
+      <c r="A19" s="16">
         <v>43862</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1068,14 +1077,28 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
+    <row r="20" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A20" s="16">
+        <v>43867</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>

</xml_diff>

<commit_message>
updated diary entry 2/10 (#301)
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/SWE265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15993992-5B2E-8945-ABA3-157011BAF1CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C77C84-4974-8545-9C37-B428A5A3FA88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>I found that going thorugh the codebase to find essential features was much easier now that I was familiar with the program. It was nice knowing where to search and using call graphs to sift through relveant methods and classes</t>
+  </si>
+  <si>
+    <t>Mental Simulations, walking through code</t>
+  </si>
+  <si>
+    <t>We learned new methods for thining in different mental models and walking through code in an efficient manner</t>
+  </si>
+  <si>
+    <t>I really liked the guest speaker - he opened me up on how you can really reuse your own software to sell to new clients. I also enjoyed walking through code and exteranlizing my thoughts to my partner during the code exercises. Shows that you can have an idea about how something works but communicating it is a whole different matter</t>
   </si>
 </sst>
 </file>
@@ -393,11 +402,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -719,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -730,24 +739,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
@@ -1046,7 +1055,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A19" s="17">
+      <c r="A19" s="16">
         <v>43862</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1068,14 +1077,28 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
+    <row r="20" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A20" s="16">
+        <v>43867</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>

</xml_diff>

<commit_message>
new diary entries 2/17
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/SWE265/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/swe265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C77C84-4974-8545-9C37-B428A5A3FA88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3829D6B2-3D26-4B42-848B-4F2C80B16D12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -211,6 +211,27 @@
   </si>
   <si>
     <t>I really liked the guest speaker - he opened me up on how you can really reuse your own software to sell to new clients. I also enjoyed walking through code and exteranlizing my thoughts to my partner during the code exercises. Shows that you can have an idea about how something works but communicating it is a whole different matter</t>
+  </si>
+  <si>
+    <t>big picture and more key expert practices</t>
+  </si>
+  <si>
+    <t>We learned about various stakeholders important to the development of software and how experts work along different levels of abstrction and how they prioritize work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I really found the key expert practice "do something else" very helpful. Often I get stuck on trying to understand how a piece of code works and I will fixate on it. I think I needed to hear that it's good practice to stop and search other areas of the code or to do somethin entirely different while your mind sorts out hte problem. </t>
+  </si>
+  <si>
+    <t>3:00 - 7:30pm</t>
+  </si>
+  <si>
+    <t>Worked on finding the stakeholders for latest project</t>
+  </si>
+  <si>
+    <t>we were able to accomplish our goal of finding stakeholders by searching thorugh forums, github, and documentation</t>
+  </si>
+  <si>
+    <t>I learned the value of documentation, forums, and github. We were lucky to have such an engaged community with our OS project. By searching through forums we learned that our OS project is actively engaged with its users by implementnig features and reporting/fixing bugs. It was great to see such an active role from the developr side and makes me appreciate how much care goes into someones software</t>
   </si>
 </sst>
 </file>
@@ -728,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:G20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1100,22 +1121,48 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+    <row r="21" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
+        <v>43874</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
+        <v>43877</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New diary 2/17 (#329)
* updated diary entry 2/10

* new diary entries 2/17

* removed temp excel file
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/SWE265/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/swe265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C77C84-4974-8545-9C37-B428A5A3FA88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3829D6B2-3D26-4B42-848B-4F2C80B16D12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -211,6 +211,27 @@
   </si>
   <si>
     <t>I really liked the guest speaker - he opened me up on how you can really reuse your own software to sell to new clients. I also enjoyed walking through code and exteranlizing my thoughts to my partner during the code exercises. Shows that you can have an idea about how something works but communicating it is a whole different matter</t>
+  </si>
+  <si>
+    <t>big picture and more key expert practices</t>
+  </si>
+  <si>
+    <t>We learned about various stakeholders important to the development of software and how experts work along different levels of abstrction and how they prioritize work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I really found the key expert practice "do something else" very helpful. Often I get stuck on trying to understand how a piece of code works and I will fixate on it. I think I needed to hear that it's good practice to stop and search other areas of the code or to do somethin entirely different while your mind sorts out hte problem. </t>
+  </si>
+  <si>
+    <t>3:00 - 7:30pm</t>
+  </si>
+  <si>
+    <t>Worked on finding the stakeholders for latest project</t>
+  </si>
+  <si>
+    <t>we were able to accomplish our goal of finding stakeholders by searching thorugh forums, github, and documentation</t>
+  </si>
+  <si>
+    <t>I learned the value of documentation, forums, and github. We were lucky to have such an engaged community with our OS project. By searching through forums we learned that our OS project is actively engaged with its users by implementnig features and reporting/fixing bugs. It was great to see such an active role from the developr side and makes me appreciate how much care goes into someones software</t>
   </si>
 </sst>
 </file>
@@ -728,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:G20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1100,22 +1121,48 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+    <row r="21" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
+        <v>43874</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
+        <v>43877</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated diary entries 3-13
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/swe265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD47267-F45E-1343-B5C4-78901B7DBC45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0797FA16-A6B3-1445-B3A2-1153B9D48181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -262,6 +262,24 @@
   </si>
   <si>
     <t>The example of the ducks and using "strategy" design was really helpful in udnerstanding desing patterns. I especially got a lot of value out of the link that contained the 21 or so design patterns. I feel like this is going to be really helpful to learn and try to reognize thiese patterns as I move further in my career</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Advancd topics</t>
+  </si>
+  <si>
+    <t>Learned how testing can be used to gain an undestanding of codebase</t>
+  </si>
+  <si>
+    <t>We learned a ton of concepts in Jones' class about testing and now that I'm familiar with what to look for….actaully doing the Pacman activitiy and reading the test cases really made me realize the value testing has on understanding key componenets to software. It was great because this is probably the first thing Im gonig to do in my internship to learn about the compan'ys codebase. Also, the guest speakers were awesome. They made me want to really explore my passion and I hope one day to be as inspirational as them</t>
+  </si>
+  <si>
+    <t>Important to keep a good attitude and to always learn to stay releavant and advance in your career</t>
+  </si>
+  <si>
+    <t>Jve learned a lot from this class and a key takeway for me is to always keep learning new things, perspectives, mental models. Im inspired to continue to learn new ways to challenge myself. Ill probably reach out to Andre or Kaj in the future about what are good resources to keep learning about software</t>
   </si>
 </sst>
 </file>
@@ -779,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1264,23 +1282,51 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8"/>
+    <row r="26" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+      <c r="A26" s="16">
+        <v>43895</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A27" s="16">
+        <v>43902</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>

</xml_diff>

<commit_message>
new diary entry 3-14
</commit_message>
<xml_diff>
--- a/diaries/diary-nicolas-grantham.xlsx
+++ b/diaries/diary-nicolas-grantham.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nicolas/Desktop/swe265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0797FA16-A6B3-1445-B3A2-1153B9D48181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C26F8D6-B87B-F647-B166-631D626B35B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -280,6 +280,18 @@
   </si>
   <si>
     <t>Jve learned a lot from this class and a key takeway for me is to always keep learning new things, perspectives, mental models. Im inspired to continue to learn new ways to challenge myself. Ill probably reach out to Andre or Kaj in the future about what are good resources to keep learning about software</t>
+  </si>
+  <si>
+    <t>Seond Pull Request and Test Cases</t>
+  </si>
+  <si>
+    <t>We were able to create a pull request for a second issue that we found, we documented existing test cases, we then created new test cases</t>
+  </si>
+  <si>
+    <t>I almost wish we looked at the test cases when we first dove into this project because I found a lot of valuable information about the game logic and how pieces/tiles are arranged in the game. I think moving forward when I learn a new code-base, the test cases will be the first place that I start</t>
+  </si>
+  <si>
+    <t>2:00 - 7:00</t>
   </si>
 </sst>
 </file>
@@ -797,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1328,14 +1340,28 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
+    <row r="28" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A28" s="16">
+        <v>43904</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>

</xml_diff>